<commit_message>
1) Updating the BOMs to include pricing and unifying passive MFG sources (samsung resistors).
</commit_message>
<xml_diff>
--- a/Hardware/LAB-DEB429A/docs/ADC-ClockCalculations.xlsx
+++ b/Hardware/LAB-DEB429A/docs/ADC-ClockCalculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="0" windowWidth="21480" windowHeight="9810"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="21480" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,8 +494,8 @@
         <v>2000000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C37" si="1">(7)*(10^-12)</f>
-        <v>7.0000000000000001E-12</v>
+        <f t="shared" ref="C3:C37" si="1">(17.5)*(10^-12)</f>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D37" si="2">LN(2^14)</f>
@@ -515,11 +515,11 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K37" si="3">((H3-0.5)/(B3*C3*D3))-G3</f>
-        <v>12401.722460318411</v>
+        <v>1360.6889841273633</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L37" si="4">((I3-0.5)/(B3*C3*D3))-G3</f>
-        <v>100729.99026984678</v>
+        <v>36691.996107938707</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N37" si="5">(12+H3)/B3</f>
@@ -530,11 +530,11 @@
         <v>1.3499999999999999E-5</v>
       </c>
       <c r="P3">
-        <f>(1/N3)/1000000</f>
+        <f t="shared" ref="P3:P37" si="7">(1/N3)/1000000</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q37" si="7">(1/O3)/1000000</f>
+        <f t="shared" ref="Q3:Q37" si="8">(1/O3)/1000000</f>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
@@ -568,11 +568,11 @@
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
-        <v>6267.8149735456082</v>
+        <v>-1092.8740105817569</v>
       </c>
       <c r="L4">
         <f t="shared" si="4"/>
-        <v>65153.326846564523</v>
+        <v>22461.330738625809</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
@@ -583,11 +583,11 @@
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="P4">
-        <f>(1/N4)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
@@ -621,11 +621,11 @@
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>3200.8612301592057</v>
+        <v>-2319.6555079363184</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>47364.995134923389</v>
+        <v>15345.998053969353</v>
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
@@ -636,11 +636,11 @@
         <v>6.7499999999999997E-6</v>
       </c>
       <c r="P5">
-        <f>(1/N5)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14814814814814814</v>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
@@ -674,11 +674,11 @@
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>1360.688984127366</v>
+        <v>-3055.7244063490539</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>36691.996107938721</v>
+        <v>11076.798443175485</v>
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
@@ -689,11 +689,11 @@
         <v>5.4E-6</v>
       </c>
       <c r="P6">
-        <f>(1/N6)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1851851851851852</v>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
@@ -727,11 +727,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>133.90748677280408</v>
+        <v>-3546.4370052908785</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>29576.663423282262</v>
+        <v>8230.6653693129047</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
@@ -742,11 +742,11 @@
         <v>4.5000000000000001E-6</v>
       </c>
       <c r="P7">
-        <f>(1/N7)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.22222222222222221</v>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
@@ -780,11 +780,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>-742.36501133759612</v>
+        <v>-3896.9460045350384</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>24494.282934241939</v>
+        <v>6197.7131736967767</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
@@ -795,11 +795,11 @@
         <v>3.857142857142857E-6</v>
       </c>
       <c r="P8">
-        <f>(1/N8)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25925925925925924</v>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
@@ -833,11 +833,11 @@
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>-1399.5693849203972</v>
+        <v>-4159.8277539681594</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>20682.497567461694</v>
+        <v>4672.9990269846767</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
@@ -848,11 +848,11 @@
         <v>3.3749999999999999E-6</v>
       </c>
       <c r="P9">
-        <f>(1/N9)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29629629629629628</v>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
@@ -886,11 +886,11 @@
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>-1910.7283421514639</v>
+        <v>-4364.2913368605859</v>
       </c>
       <c r="L10">
         <f t="shared" si="4"/>
-        <v>17717.775615521507</v>
+        <v>3487.1102462086037</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
@@ -901,11 +901,11 @@
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="P10">
-        <f>(1/N10)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
@@ -939,11 +939,11 @@
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>-2319.655507936317</v>
+        <v>-4527.8622031745272</v>
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>15345.998053969361</v>
+        <v>2538.3992215877424</v>
       </c>
       <c r="N11">
         <f t="shared" si="5"/>
@@ -954,11 +954,11 @@
         <v>2.7E-6</v>
       </c>
       <c r="P11">
-        <f>(1/N11)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.37037037037037041</v>
       </c>
     </row>
@@ -972,7 +972,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
@@ -992,11 +992,11 @@
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>-2654.2322799421067</v>
+        <v>-4661.6929119768429</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>13405.45277633578</v>
+        <v>1762.1811105343104</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
@@ -1007,11 +1007,11 @@
         <v>2.4545454545454544E-6</v>
       </c>
       <c r="P12">
-        <f>(1/N12)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.73333333333333339</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.40740740740740744</v>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
@@ -1045,11 +1045,11 @@
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>-2933.046256613598</v>
+        <v>-4773.218502645439</v>
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>11788.331711641131</v>
+        <v>1115.3326846564523</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
@@ -1060,11 +1060,11 @@
         <v>2.2500000000000001E-6</v>
       </c>
       <c r="P13">
-        <f>(1/N13)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.44444444444444442</v>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
@@ -1098,11 +1098,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>-3168.9657753356287</v>
+        <v>-4867.5863101342511</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>10419.998503053353</v>
+        <v>567.99940122134103</v>
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
@@ -1113,11 +1113,11 @@
         <v>2.0769230769230768E-6</v>
       </c>
       <c r="P14">
-        <f>(1/N14)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.86666666666666659</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.48148148148148151</v>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
@@ -1151,11 +1151,11 @@
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>-3371.1825056687981</v>
+        <v>-4948.4730022675194</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>9247.1414671209695</v>
+        <v>98.856586848388361</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
@@ -1166,11 +1166,11 @@
         <v>1.9285714285714285E-6</v>
       </c>
       <c r="P15">
-        <f>(1/N15)/1000000</f>
+        <f t="shared" si="7"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.51851851851851849</v>
       </c>
     </row>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
@@ -1204,11 +1204,11 @@
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>-3546.4370052908785</v>
+        <v>-5018.5748021163517</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>8230.6653693129047</v>
+        <v>-307.73385227483868</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
@@ -1219,11 +1219,11 @@
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="P16">
-        <f>(1/N16)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.55555555555555558</v>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
@@ -1257,11 +1257,11 @@
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>-3699.7846924601986</v>
+        <v>-5079.9138769840793</v>
       </c>
       <c r="L17">
         <f t="shared" si="4"/>
-        <v>7341.2487837308472</v>
+        <v>-663.50048650766166</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
@@ -1272,11 +1272,11 @@
         <v>1.6874999999999999E-6</v>
       </c>
       <c r="P17">
-        <f>(1/N17)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.0666666666666667</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.59259259259259256</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
@@ -1310,11 +1310,11 @@
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
-        <v>-3835.0914752566573</v>
+        <v>-5134.0365901026635</v>
       </c>
       <c r="L18">
         <f t="shared" si="4"/>
-        <v>6556.469443511387</v>
+        <v>-977.41222259544611</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
@@ -1325,11 +1325,11 @@
         <v>1.588235294117647E-6</v>
       </c>
       <c r="P18">
-        <f>(1/N18)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.1333333333333333</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.62962962962962965</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
@@ -1363,11 +1363,11 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>-3955.364171075732</v>
+        <v>-5182.145668430293</v>
       </c>
       <c r="L19">
         <f t="shared" si="4"/>
-        <v>5858.8878077607533</v>
+        <v>-1256.4448768956981</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
@@ -1378,11 +1378,11 @@
         <v>1.5E-6</v>
       </c>
       <c r="P19">
-        <f>(1/N19)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.2</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
@@ -1416,11 +1416,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>-4062.9765831243776</v>
+        <v>-5225.190633249751</v>
       </c>
       <c r="L20">
         <f t="shared" si="4"/>
-        <v>5234.7358178786089</v>
+        <v>-1506.1056728485564</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
@@ -1431,11 +1431,11 @@
         <v>1.4210526315789473E-6</v>
       </c>
       <c r="P20">
-        <f>(1/N20)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.2666666666666668</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.70370370370370372</v>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
@@ -1469,11 +1469,11 @@
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>-4159.8277539681585</v>
+        <v>-5263.9311015872636</v>
       </c>
       <c r="L21">
         <f t="shared" si="4"/>
-        <v>4672.9990269846803</v>
+        <v>-1730.8003892061288</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
@@ -1484,11 +1484,11 @@
         <v>1.35E-6</v>
       </c>
       <c r="P21">
-        <f>(1/N21)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.74074074074074081</v>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D22">
         <f t="shared" si="2"/>
@@ -1522,11 +1522,11 @@
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
-        <v>-4247.4550037791987</v>
+        <v>-5298.9820015116793</v>
       </c>
       <c r="L22">
         <f t="shared" si="4"/>
-        <v>4164.760978080647</v>
+        <v>-1934.0956087677419</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
@@ -1537,11 +1537,11 @@
         <v>1.2857142857142858E-6</v>
       </c>
       <c r="P22">
-        <f>(1/N22)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.4</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.77777777777777779</v>
       </c>
     </row>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
@@ -1575,11 +1575,11 @@
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>-4327.1161399710536</v>
+        <v>-5330.8464559884214</v>
       </c>
       <c r="L23">
         <f t="shared" si="4"/>
-        <v>3702.72638816789</v>
+        <v>-2118.9094447328448</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
@@ -1590,11 +1590,11 @@
         <v>1.2272727272727272E-6</v>
       </c>
       <c r="P23">
-        <f>(1/N23)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.4666666666666668</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.81481481481481488</v>
       </c>
     </row>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
@@ -1628,11 +1628,11 @@
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
-        <v>-4399.8502208418777</v>
+        <v>-5359.9400883367507</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
-        <v>3280.8687191171102</v>
+        <v>-2287.6525123531555</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
@@ -1643,11 +1643,11 @@
         <v>1.1739130434782609E-6</v>
       </c>
       <c r="P24">
-        <f>(1/N24)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.5333333333333332</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.85185185185185175</v>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
@@ -1681,11 +1681,11 @@
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
-        <v>-4466.5231283067988</v>
+        <v>-5386.6092513227195</v>
       </c>
       <c r="L25">
         <f t="shared" si="4"/>
-        <v>2894.1658558205654</v>
+        <v>-2442.3336576717738</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
@@ -1696,11 +1696,11 @@
         <v>1.125E-6</v>
       </c>
       <c r="P25">
-        <f>(1/N25)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.5999999999999999</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
@@ -1734,11 +1734,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>-4527.8622031745272</v>
+        <v>-5411.1448812698109</v>
       </c>
       <c r="L26">
         <f t="shared" si="4"/>
-        <v>2538.3992215877424</v>
+        <v>-2584.6403113649026</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
@@ -1749,11 +1749,11 @@
         <v>1.08E-6</v>
       </c>
       <c r="P26">
-        <f>(1/N26)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.92592592592592582</v>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
@@ -1787,11 +1787,11 @@
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
-        <v>-4584.4828876678148</v>
+        <v>-5433.7931550671256</v>
       </c>
       <c r="L27">
         <f t="shared" si="4"/>
-        <v>2209.9992515266767</v>
+        <v>-2716.0002993893295</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
@@ -1802,11 +1802,11 @@
         <v>1.0384615384615384E-6</v>
       </c>
       <c r="P27">
-        <f>(1/N27)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.7333333333333332</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.96296296296296302</v>
       </c>
     </row>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
@@ -1840,11 +1840,11 @@
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
-        <v>-4636.9094473838213</v>
+        <v>-5454.7637789535283</v>
       </c>
       <c r="L28">
         <f t="shared" si="4"/>
-        <v>1905.9252051738358</v>
+        <v>-2837.6299179304656</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
@@ -1855,11 +1855,11 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="P28">
-        <f>(1/N28)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.8000000000000003</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
@@ -1893,11 +1893,11 @@
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
-        <v>-4685.5912528343988</v>
+        <v>-5474.2365011337597</v>
       </c>
       <c r="L29">
         <f t="shared" si="4"/>
-        <v>1623.5707335604848</v>
+        <v>-2950.5717065758058</v>
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
@@ -1908,11 +1908,11 @@
         <v>9.6428571428571425E-7</v>
       </c>
       <c r="P29">
-        <f>(1/N29)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.8666666666666667</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.037037037037037</v>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
@@ -1946,11 +1946,11 @@
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>-4730.9156923918335</v>
+        <v>-5492.3662769567336</v>
       </c>
       <c r="L30">
         <f t="shared" si="4"/>
-        <v>1360.6889841273651</v>
+        <v>-3055.7244063490543</v>
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
@@ -1961,11 +1961,11 @@
         <v>9.3103448275862071E-7</v>
       </c>
       <c r="P30">
-        <f>(1/N30)/1000000</f>
+        <f t="shared" si="7"/>
         <v>1.9333333333333336</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0740740740740742</v>
       </c>
     </row>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
@@ -1999,11 +1999,11 @@
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
-        <v>-4773.218502645439</v>
+        <v>-5509.2874010581754</v>
       </c>
       <c r="L31">
         <f t="shared" si="4"/>
-        <v>1115.3326846564523</v>
+        <v>-3153.8669261374193</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
@@ -2014,11 +2014,11 @@
         <v>8.9999999999999996E-7</v>
       </c>
       <c r="P31">
-        <f>(1/N31)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1111111111111112</v>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
@@ -2052,11 +2052,11 @@
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
-        <v>-4812.7920993342959</v>
+        <v>-5525.1168397337187</v>
       </c>
       <c r="L32">
         <f t="shared" si="4"/>
-        <v>885.80582386108381</v>
+        <v>-3245.6776704555668</v>
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
@@ -2067,11 +2067,11 @@
         <v>8.7096774193548392E-7</v>
       </c>
       <c r="P32">
-        <f>(1/N32)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.0666666666666664</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1481481481481481</v>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
@@ -2105,11 +2105,11 @@
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
-        <v>-4849.8923462300991</v>
+        <v>-5539.9569384920396</v>
       </c>
       <c r="L33">
         <f t="shared" si="4"/>
-        <v>670.6243918654236</v>
+        <v>-3331.7502432538308</v>
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
@@ -2120,11 +2120,11 @@
         <v>8.4374999999999997E-7</v>
       </c>
       <c r="P33">
-        <f>(1/N33)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.1333333333333333</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1851851851851851</v>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
@@ -2158,11 +2158,11 @@
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
-        <v>-4884.7440933140351</v>
+        <v>-5553.8976373256146</v>
       </c>
       <c r="L34">
         <f t="shared" si="4"/>
-        <v>468.48425877859336</v>
+        <v>-3412.6062964885627</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
@@ -2173,11 +2173,11 @@
         <v>8.1818181818181823E-7</v>
       </c>
       <c r="P34">
-        <f>(1/N34)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
@@ -2211,11 +2211,11 @@
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
-        <v>-4917.5457376283284</v>
+        <v>-5567.0182950513317</v>
       </c>
       <c r="L35">
         <f t="shared" si="4"/>
-        <v>278.2347217556935</v>
+        <v>-3488.7061112977231</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
@@ -2226,11 +2226,11 @@
         <v>7.9411764705882348E-7</v>
       </c>
       <c r="P35">
-        <f>(1/N35)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.2666666666666666</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2592592592592593</v>
       </c>
     </row>
@@ -2244,7 +2244,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
@@ -2264,11 +2264,11 @@
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
-        <v>-4948.4730022675194</v>
+        <v>-5579.3892009070078</v>
       </c>
       <c r="L36">
         <f t="shared" si="4"/>
-        <v>98.856586848388361</v>
+        <v>-3560.457365260645</v>
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
@@ -2279,11 +2279,11 @@
         <v>7.7142857142857138E-7</v>
       </c>
       <c r="P36">
-        <f>(1/N36)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2962962962962965</v>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-12</v>
+        <v>1.7500000000000001E-11</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
@@ -2317,11 +2317,11 @@
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
-        <v>-4977.6820855378664</v>
+        <v>-5591.072834215146</v>
       </c>
       <c r="L37">
         <f t="shared" si="4"/>
-        <v>-70.556096119623362</v>
+        <v>-3628.2224384478491</v>
       </c>
       <c r="N37">
         <f t="shared" si="5"/>
@@ -2332,11 +2332,11 @@
         <v>7.5000000000000002E-7</v>
       </c>
       <c r="P37">
-        <f>(1/N37)/1000000</f>
+        <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.3333333333333333</v>
       </c>
     </row>

</xml_diff>